<commit_message>
renamed project in GPL preambles
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="162">
   <si>
     <t>t</t>
   </si>
@@ -46,15 +46,6 @@
     <t>RunSimulator</t>
   </si>
   <si>
-    <t>..\ExcelReader\bin\Debug\ExcelReader.exe</t>
-  </si>
-  <si>
-    <t>..\..\SolarLoadModel\SolarLoadModel\bin\Debug\SolarLoadModel.exe</t>
-  </si>
-  <si>
-    <t>..\..\SolarLoadModel\Data</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
@@ -205,12 +196,6 @@
     <t>Gen8IdealPctP</t>
   </si>
   <si>
-    <t>Log File</t>
-  </si>
-  <si>
-    <t>log_entries.txt</t>
-  </si>
-  <si>
     <t>analyse.csv</t>
   </si>
   <si>
@@ -220,9 +205,6 @@
     <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
   </si>
   <si>
-    <t>GenConfig*</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -493,15 +475,6 @@
     <t>Percent Complete</t>
   </si>
   <si>
-    <t>Watch</t>
-  </si>
-  <si>
-    <t>watchfile.txt</t>
-  </si>
-  <si>
-    <t>Run 172800 iterations...</t>
-  </si>
-  <si>
     <t>load.csv</t>
   </si>
   <si>
@@ -514,31 +487,25 @@
     <t>NPV Analyser.xls</t>
   </si>
   <si>
-    <t>*MaxP</t>
-  </si>
-  <si>
-    <t>*SetP</t>
-  </si>
-  <si>
-    <t>*Cfg</t>
-  </si>
-  <si>
-    <t>*Pa</t>
-  </si>
-  <si>
-    <t>Gen[1-4]StartCnt</t>
-  </si>
-  <si>
     <t>GenAvailSet</t>
   </si>
   <si>
-    <t>Run started on 25/02/2013 8:21:13 AM</t>
-  </si>
-  <si>
-    <t>version 2013/02/22-20662</t>
-  </si>
-  <si>
-    <t>inner loop took 1.70017s</t>
+    <t>C:\Program Files (x86)\Power Water Corporation\Asim\AsimExcelTools.exe</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\Power Water Corporation\Asim\Asim.exe</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Run started on 15/03/2013 3:38:17 PM</t>
+  </si>
+  <si>
+    <t>version 2013/03/15-28043</t>
+  </si>
+  <si>
+    <t>inner loop took 1.4211421s</t>
   </si>
 </sst>
 </file>
@@ -723,11 +690,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186153984"/>
-        <c:axId val="185996032"/>
+        <c:axId val="154995712"/>
+        <c:axId val="155054848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186153984"/>
+        <c:axId val="154995712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -739,12 +706,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185996032"/>
+        <c:crossAx val="155054848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185996032"/>
+        <c:axId val="155054848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186153984"/>
+        <c:crossAx val="154995712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -786,10 +753,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -835,11 +798,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="61489152"/>
-        <c:axId val="61490688"/>
+        <c:axId val="155778432"/>
+        <c:axId val="155937024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61489152"/>
+        <c:axId val="155778432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61490688"/>
+        <c:crossAx val="155937024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -856,7 +819,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61490688"/>
+        <c:axId val="155937024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -869,7 +832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61489152"/>
+        <c:crossAx val="155778432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -938,7 +901,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1244,10 +1207,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,40 +1226,40 @@
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="B4" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B5" s="8">
         <v>41196.600694444445</v>
@@ -1304,7 +1267,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1312,102 +1275,68 @@
         <v>172800</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C9">
         <v>604800</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E12" t="s">
-        <v>166</v>
-      </c>
-      <c r="F12" t="s">
-        <v>167</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations disablePrompts="1" count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
     </dataValidation>
@@ -1423,17 +1352,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2">
       <formula1>",,,,,Community Name,,,input,output,,FlattenApplication"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
-      <formula1>",,,,,Community Name,Template,,input,output,,,Log File"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
-      <formula1>",,,,,Community Name,Template,,input,output,,,Watch"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,Template,,input,output,,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
       <formula1>",,,,,Community Name,,,input,output,,,Parameter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
+      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1466,85 +1392,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>169</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="U1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>54</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>55</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>57</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -1658,244 +1584,244 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>78</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>79</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>80</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>81</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>82</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>84</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>85</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>86</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>87</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>88</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>89</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AC1" t="s">
         <v>90</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AD1" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>92</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
         <v>93</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AG1" t="s">
         <v>94</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AH1" t="s">
         <v>95</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AI1" t="s">
         <v>96</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AJ1" t="s">
         <v>97</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AK1" t="s">
         <v>98</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AL1" t="s">
         <v>99</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AM1" t="s">
         <v>100</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AN1" t="s">
         <v>101</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AO1" t="s">
         <v>102</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AP1" t="s">
         <v>103</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AQ1" t="s">
         <v>104</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AR1" t="s">
         <v>105</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AS1" t="s">
         <v>106</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AT1" t="s">
         <v>107</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AU1" t="s">
         <v>108</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AV1" t="s">
         <v>109</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AW1" t="s">
         <v>110</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AX1" t="s">
         <v>111</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AY1" t="s">
         <v>112</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AZ1" t="s">
         <v>113</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BA1" t="s">
         <v>114</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BB1" t="s">
         <v>115</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BC1" t="s">
         <v>116</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BD1" t="s">
         <v>117</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BE1" t="s">
         <v>118</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BF1" t="s">
         <v>119</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BG1" t="s">
         <v>120</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BH1" t="s">
         <v>121</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BI1" t="s">
         <v>122</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BJ1" t="s">
         <v>123</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BK1" t="s">
         <v>124</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BL1" t="s">
         <v>125</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BM1" t="s">
         <v>126</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BN1" t="s">
         <v>127</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BO1" t="s">
         <v>128</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BP1" t="s">
         <v>129</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BQ1" t="s">
         <v>130</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BR1" t="s">
         <v>131</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BS1" t="s">
         <v>132</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BT1" t="s">
         <v>133</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BU1" t="s">
         <v>134</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BV1" t="s">
         <v>135</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BW1" t="s">
         <v>136</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BX1" t="s">
         <v>137</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BY1" t="s">
         <v>138</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BZ1" t="s">
         <v>139</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CA1" t="s">
         <v>140</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CB1" t="s">
         <v>141</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CC1" t="s">
         <v>142</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>143</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>144</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>145</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>146</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>147</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
@@ -2166,10 +2092,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2206,61 +2132,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>38</v>
-      </c>
-      <c r="R1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2356,10 +2282,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2381,7 +2307,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -2391,60 +2317,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>172</v>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of fixes with renaming, publishing, exe locations, new example spreadsheets, macros, etc.
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="158">
   <si>
     <t>t</t>
   </si>
@@ -28,15 +28,9 @@
     <t>config</t>
   </si>
   <si>
-    <t>FlattenApplication</t>
-  </si>
-  <si>
     <t>iterations</t>
   </si>
   <si>
-    <t>Simulator</t>
-  </si>
-  <si>
     <t>directory</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Solar Load Model  Copyright (C) 2012, 2013  Power Water Corporation.</t>
-  </si>
-  <si>
     <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
   </si>
   <si>
@@ -490,22 +481,19 @@
     <t>GenAvailSet</t>
   </si>
   <si>
-    <t>C:\Program Files (x86)\Power Water Corporation\Asim\AsimExcelTools.exe</t>
-  </si>
-  <si>
-    <t>C:\Program Files (x86)\Power Water Corporation\Asim\Asim.exe</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
-    <t>Run started on 15/03/2013 3:38:17 PM</t>
-  </si>
-  <si>
-    <t>version 2013/03/15-28043</t>
-  </si>
-  <si>
-    <t>inner loop took 1.4211421s</t>
+    <t>Asim  Copyright (C) 2012, 2013  Power Water Corporation.</t>
+  </si>
+  <si>
+    <t>Run started on 18/03/2013 9:39:41 AM</t>
+  </si>
+  <si>
+    <t>version 2013/03/18-17327</t>
+  </si>
+  <si>
+    <t>inner loop took 3.5313531s</t>
   </si>
 </sst>
 </file>
@@ -690,11 +678,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="154995712"/>
-        <c:axId val="155054848"/>
+        <c:axId val="127868288"/>
+        <c:axId val="127919232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154995712"/>
+        <c:axId val="127868288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -706,12 +694,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155054848"/>
+        <c:crossAx val="127919232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="155054848"/>
+        <c:axId val="127919232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +710,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154995712"/>
+        <c:crossAx val="127868288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -798,11 +786,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="155778432"/>
-        <c:axId val="155937024"/>
+        <c:axId val="128412672"/>
+        <c:axId val="128414464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="155778432"/>
+        <c:axId val="128412672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155937024"/>
+        <c:crossAx val="128414464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -819,7 +807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155937024"/>
+        <c:axId val="128414464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -832,7 +820,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155778432"/>
+        <c:crossAx val="128412672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1207,11 +1195,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1234,48 +1220,50 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>156</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>157</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B3" s="8">
+        <v>41196.600694444445</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>172800</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="8">
-        <v>41196.600694444445</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7">
-        <v>172800</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>143</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1283,83 +1271,62 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>604800</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9">
-        <v>604800</v>
-      </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>148</v>
+        <v>151</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
+      <c r="B10" s="7"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A4">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A3">
       <formula1>",,,,,,,,input,output,Start Time,Community Name"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B8">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A7">
       <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2">
-      <formula1>",,,,,Community Name,,,input,output,,FlattenApplication"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
+      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
-      <formula1>",,,,,Community Name,Template,,input,output,,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A10">
+      <formula1>"FlattenApplication,Simulator,,,,Community Name,Template,Log File,input,output,,Watch,Parameter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
-      <formula1>",,,,,Community Name,,,input,output,,,Parameter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
-      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
+      <formula1>"FlattenApplication,Simulator,,,,Community Name,Template,Log File,input,output,,Watch,Parameter"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1392,85 +1359,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="U1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" t="s">
         <v>50</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>51</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>55</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -1584,244 +1551,244 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>72</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>73</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>74</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>76</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>78</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>79</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>81</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>82</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>83</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>84</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>85</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>87</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>88</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>89</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>90</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>91</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>92</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>93</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>94</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>95</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>96</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>97</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>99</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>101</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>102</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>103</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>104</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>105</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>106</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>107</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>108</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>109</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>110</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>111</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>112</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>113</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>114</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>115</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>116</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>117</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>118</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>119</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>120</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BJ1" t="s">
         <v>121</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BK1" t="s">
         <v>122</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BL1" t="s">
         <v>123</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BM1" t="s">
         <v>124</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BN1" t="s">
         <v>125</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BO1" t="s">
         <v>126</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BP1" t="s">
         <v>127</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BQ1" t="s">
         <v>128</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BR1" t="s">
         <v>129</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BS1" t="s">
         <v>130</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BT1" t="s">
         <v>131</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>132</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" t="s">
         <v>133</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BW1" t="s">
         <v>134</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BX1" t="s">
         <v>135</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BY1" t="s">
         <v>136</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BZ1" t="s">
         <v>137</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CA1" t="s">
         <v>138</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CB1" t="s">
         <v>139</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CC1" t="s">
         <v>140</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>141</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
@@ -2092,10 +2059,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2132,61 +2099,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
-      </c>
-      <c r="S1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2282,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2317,47 +2284,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
@@ -2365,7 +2332,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Example spreadsheets with better defaults.
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
   <si>
     <t>t</t>
   </si>
@@ -448,24 +448,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
-  </si>
-  <si>
-    <t>This is free software, and you are welcome to redistribute it</t>
-  </si>
-  <si>
-    <t>under certain conditions; see the file COPYING for details.</t>
-  </si>
-  <si>
     <t>*E</t>
   </si>
   <si>
-    <t>Init...</t>
-  </si>
-  <si>
-    <t>Percent Complete</t>
-  </si>
-  <si>
     <t>load.csv</t>
   </si>
   <si>
@@ -484,16 +469,19 @@
     <t>.</t>
   </si>
   <si>
-    <t>Asim  Copyright (C) 2012, 2013  Power Water Corporation.</t>
-  </si>
-  <si>
-    <t>Run started on 18/03/2013 9:39:41 AM</t>
-  </si>
-  <si>
-    <t>version 2013/03/18-17327</t>
-  </si>
-  <si>
-    <t>inner loop took 3.5313531s</t>
+    <t>LoadCapMargin</t>
+  </si>
+  <si>
+    <t>FlattenApplication</t>
+  </si>
+  <si>
+    <t>bin\ExcelReader.exe</t>
+  </si>
+  <si>
+    <t>Simulator</t>
+  </si>
+  <si>
+    <t>bin\SolarLoadModel.exe</t>
   </si>
 </sst>
 </file>
@@ -601,6 +589,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -678,11 +667,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127868288"/>
-        <c:axId val="127919232"/>
+        <c:axId val="146369536"/>
+        <c:axId val="146400000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127868288"/>
+        <c:axId val="146369536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -694,12 +683,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127919232"/>
+        <c:crossAx val="146400000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127919232"/>
+        <c:axId val="146400000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127868288"/>
+        <c:crossAx val="146369536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -741,6 +730,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -756,9 +749,6 @@
               <c:f>SimResults!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Percent Complete</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -769,9 +759,6 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -786,11 +773,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="128412672"/>
-        <c:axId val="128414464"/>
+        <c:axId val="146647296"/>
+        <c:axId val="146653184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128412672"/>
+        <c:axId val="146647296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128414464"/>
+        <c:crossAx val="146653184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -807,7 +794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128414464"/>
+        <c:axId val="146653184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -820,7 +807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128412672"/>
+        <c:crossAx val="146647296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1195,7 +1182,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1220,29 +1207,29 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="8">
-        <v>41196.600694444445</v>
+        <v>152</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7">
-        <v>172800</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>141</v>
@@ -1250,28 +1237,28 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>148</v>
+        <v>60</v>
+      </c>
+      <c r="B5" s="8">
+        <v>41196.600694444445</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>149</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="7">
+        <v>172800</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>56</v>
+        <v>143</v>
       </c>
       <c r="C7">
         <v>604800</v>
@@ -1280,53 +1267,72 @@
         <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A4">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A5">
       <formula1>",,,,,,,,input,output,Start Time,Community Name"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
       <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
       <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11:A12">
       <formula1>"FlattenApplication,Simulator,,,,Community Name,Template,Log File,input,output,,Watch,Parameter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
-      <formula1>"FlattenApplication,Simulator,,,,Community Name,Template,Log File,input,output,,Watch,Parameter"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A4">
+      <formula1>"FlattenApplication,Simulator,,,,Community Name,,Log File,input,output,,Watch,Parameter,directory"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2">
+      <formula1>",,,,,Community Name,,,input,output,,FlattenApplication"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1339,9 +1345,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1383,7 +1387,7 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>15</v>
@@ -1536,9 +1540,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:CC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2045,16 +2047,17 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2064,8 +2067,11 @@
       <c r="C1" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2074,6 +2080,9 @@
       </c>
       <c r="C2">
         <v>50</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2274,11 +2283,9 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2287,53 +2294,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>146</v>
-      </c>
-    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>157</v>
-      </c>
+      <c r="B10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated with new exe file names.
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -475,13 +475,13 @@
     <t>FlattenApplication</t>
   </si>
   <si>
-    <t>bin\ExcelReader.exe</t>
-  </si>
-  <si>
     <t>Simulator</t>
   </si>
   <si>
-    <t>bin\SolarLoadModel.exe</t>
+    <t>bin\Asim.exe</t>
+  </si>
+  <si>
+    <t>bin\AsimExcelTools.exe</t>
   </si>
 </sst>
 </file>
@@ -667,11 +667,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150563840"/>
-        <c:axId val="150405888"/>
+        <c:axId val="155429888"/>
+        <c:axId val="155198208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150563840"/>
+        <c:axId val="155429888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -683,12 +683,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150405888"/>
+        <c:crossAx val="155198208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150405888"/>
+        <c:axId val="155198208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150563840"/>
+        <c:crossAx val="155429888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -773,11 +773,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="151238912"/>
-        <c:axId val="151240704"/>
+        <c:axId val="156035328"/>
+        <c:axId val="156037120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151238912"/>
+        <c:axId val="156035328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151240704"/>
+        <c:crossAx val="156037120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -794,7 +794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151240704"/>
+        <c:axId val="156037120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -807,7 +807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151238912"/>
+        <c:crossAx val="156035328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1210,13 +1210,13 @@
         <v>150</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
fixed new file names.
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -589,7 +589,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -667,11 +666,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="155429888"/>
-        <c:axId val="155198208"/>
+        <c:axId val="150187008"/>
+        <c:axId val="149955328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="155429888"/>
+        <c:axId val="150187008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -683,12 +682,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155198208"/>
+        <c:crossAx val="149955328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="155198208"/>
+        <c:axId val="149955328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155429888"/>
+        <c:crossAx val="150187008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -731,7 +730,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -773,11 +771,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="156035328"/>
-        <c:axId val="156037120"/>
+        <c:axId val="152955136"/>
+        <c:axId val="152956928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156035328"/>
+        <c:axId val="152955136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +784,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156037120"/>
+        <c:crossAx val="152956928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -794,7 +792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156037120"/>
+        <c:axId val="152956928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -807,7 +805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156035328"/>
+        <c:crossAx val="152955136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1210,7 +1208,7 @@
         <v>150</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1219,7 +1217,7 @@
         <v>151</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>

</xml_diff>

<commit_message>
PWCSLMS-31 excel startup up wizard, new addin & xls files.
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -7,20 +7,24 @@
     <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725"/>
   </bookViews>
   <sheets>
-    <sheet name="config" sheetId="4" r:id="rId1"/>
-    <sheet name="GenStats" sheetId="1" r:id="rId2"/>
-    <sheet name="FuelEfficiency" sheetId="7" r:id="rId3"/>
-    <sheet name="StationStats" sheetId="2" r:id="rId4"/>
-    <sheet name="GenConfigurations" sheetId="3" r:id="rId5"/>
-    <sheet name="Solar" sheetId="5" r:id="rId6"/>
-    <sheet name="SimResults" sheetId="6" r:id="rId7"/>
+    <sheet name="Wizard" sheetId="8" r:id="rId1"/>
+    <sheet name="config" sheetId="4" r:id="rId2"/>
+    <sheet name="GenStats" sheetId="1" r:id="rId3"/>
+    <sheet name="FuelEfficiency" sheetId="7" r:id="rId4"/>
+    <sheet name="StationStats" sheetId="2" r:id="rId5"/>
+    <sheet name="GenConfigurations" sheetId="3" r:id="rId6"/>
+    <sheet name="Solar" sheetId="5" r:id="rId7"/>
+    <sheet name="SimResults" sheetId="6" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="168">
   <si>
     <t>t</t>
   </si>
@@ -482,6 +486,48 @@
   </si>
   <si>
     <t>bin\AsimExcelTools.exe</t>
+  </si>
+  <si>
+    <t>Hysteresis</t>
+  </si>
+  <si>
+    <t>Spinning Reserve Setpoint</t>
+  </si>
+  <si>
+    <t>Generator Minimum Run Time</t>
+  </si>
+  <si>
+    <t>Use this startup wizard to quickly fill in values in the simulation</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Generator 1 Nominal Rating</t>
+  </si>
+  <si>
+    <t>Generator 2 Nominal Rating</t>
+  </si>
+  <si>
+    <t>Generator 3 Nominal Rating</t>
+  </si>
+  <si>
+    <t>Generator 4 Nominal Rating</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -491,7 +537,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,16 +553,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -524,12 +608,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -540,12 +641,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -666,11 +798,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150187008"/>
-        <c:axId val="149955328"/>
+        <c:axId val="165102336"/>
+        <c:axId val="165103872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150187008"/>
+        <c:axId val="165102336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -682,12 +814,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149955328"/>
+        <c:crossAx val="165103872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149955328"/>
+        <c:axId val="165103872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150187008"/>
+        <c:crossAx val="165102336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -730,6 +862,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -771,11 +904,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="152955136"/>
-        <c:axId val="152956928"/>
+        <c:axId val="166592512"/>
+        <c:axId val="166594048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152955136"/>
+        <c:axId val="166592512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152956928"/>
+        <c:crossAx val="166594048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -792,7 +925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152956928"/>
+        <c:axId val="166594048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -805,7 +938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152955136"/>
+        <c:crossAx val="166592512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -822,7 +955,140 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3073" name="RunWizard" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3073"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Run Wizard</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>552450</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3075" name="RunAsim" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3075"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Run Asim</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -857,7 +1123,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -890,6 +1156,35 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="config"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="RunApplication.RunApplication"/>
+      <definedName name="StartupWizard.RunWizard"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:D11" totalsRowShown="0" headerRowCellStyle="60% - Accent1">
+  <tableColumns count="4">
+    <tableColumn id="1" name="Parameter" dataDxfId="0"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="Value"/>
+    <tableColumn id="4" name="Units"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,11 +1473,219 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7">
+        <v>3600</v>
+      </c>
+      <c r="D7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11">
+        <v>400</v>
+      </c>
+      <c r="D11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",F1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3073" r:id="rId4" name="RunWizard">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!StartupWizard.RunWizard">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3075" r:id="rId5" name="RunAsim">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!RunApplication.RunApplication">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>552450</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1248,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="7">
-        <v>172800</v>
+        <v>86400</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1338,9 +1841,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1450,13 +1953,13 @@
         <v>80</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="F2">
         <v>100</v>
@@ -1533,7 +2036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:CC2"/>
@@ -2042,12 +2545,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2088,7 +2593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T2"/>
@@ -2234,7 +2739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C2"/>
@@ -2278,7 +2783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B10"/>

</xml_diff>

<commit_message>
fixed bug with one-cell worksheets; started post-processing option PWCSLMS-28
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725"/>
+    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wizard" sheetId="8" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="176">
   <si>
     <t>t</t>
   </si>
@@ -197,9 +197,6 @@
     <t>analyse.csv</t>
   </si>
   <si>
-    <t>*Cnt</t>
-  </si>
-  <si>
     <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
   </si>
   <si>
@@ -452,18 +449,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>*E</t>
-  </si>
-  <si>
     <t>load.csv</t>
   </si>
   <si>
     <t>renewables.csv</t>
   </si>
   <si>
-    <t>Template</t>
-  </si>
-  <si>
     <t>NPV Analyser.xls</t>
   </si>
   <si>
@@ -528,6 +519,39 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Batch Command</t>
+  </si>
+  <si>
+    <t>Gen1P{max,min}</t>
+  </si>
+  <si>
+    <t>Asim  Copyright (C) 2012, 2013  Power Water Corporation.</t>
+  </si>
+  <si>
+    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
+  </si>
+  <si>
+    <t>This is free software, and you are welcome to redistribute it</t>
+  </si>
+  <si>
+    <t>under certain conditions; see the file COPYING for details.</t>
+  </si>
+  <si>
+    <t>version 2013/06/07-18880</t>
+  </si>
+  <si>
+    <t>Init...</t>
+  </si>
+  <si>
+    <t>Percent Complete</t>
+  </si>
+  <si>
+    <t>Run started on 11/06/2013 4:04:31 PM</t>
+  </si>
+  <si>
+    <t>inner loop took 1.290129s</t>
   </si>
 </sst>
 </file>
@@ -861,10 +885,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -880,6 +900,9 @@
               <c:f>SimResults!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percent Complete</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -890,6 +913,9 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -904,11 +930,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="166592512"/>
-        <c:axId val="166594048"/>
+        <c:axId val="35513088"/>
+        <c:axId val="35514624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166592512"/>
+        <c:axId val="35513088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166594048"/>
+        <c:crossAx val="35514624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -925,7 +951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166594048"/>
+        <c:axId val="35514624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -938,7 +964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166592512"/>
+        <c:crossAx val="35513088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1140,7 +1166,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1477,7 +1503,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1490,7 +1516,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1498,16 +1524,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1515,13 +1541,13 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1529,13 +1555,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C6">
         <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,13 +1569,13 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C7">
         <v>3600</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,13 +1583,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C8">
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,13 +1597,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,13 +1611,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1599,13 +1625,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C11">
         <v>400</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1683,8 +1709,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,19 +1734,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1730,15 +1756,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="8">
         <v>41196.600694444445</v>
@@ -1759,7 +1785,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1778,13 +1804,10 @@
         <v>56</v>
       </c>
       <c r="C9">
-        <v>604800</v>
+        <v>86400</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,25 +1815,25 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>145</v>
-      </c>
       <c r="B11" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>165</v>
+      </c>
       <c r="B12" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
     </dataValidation>
@@ -1820,20 +1843,23 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
-      <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
-      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11:A12">
-      <formula1>"FlattenApplication,Simulator,,,,Community Name,Template,Log File,input,output,,Watch,Parameter"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A4">
       <formula1>"FlattenApplication,Simulator,,,,Community Name,,Log File,input,output,,Watch,Parameter,directory"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2">
       <formula1>",,,,,Community Name,,,input,output,,FlattenApplication"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
+      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter,output"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
+      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
+      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter,Template"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
+      <formula1>",,,,,Community Name,Template,Log File,input,output,,Watch,Parameter,Batch Command"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1888,7 +1914,7 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>15</v>
@@ -2054,244 +2080,244 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>74</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>77</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>78</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>79</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>80</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>81</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>82</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>83</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>84</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>85</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>86</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>87</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>88</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>92</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>93</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>94</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>95</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>96</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>97</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>98</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>99</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>100</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>101</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>102</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>103</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>104</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>105</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>106</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>107</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>108</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>109</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>110</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>111</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>112</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>113</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>114</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>115</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>116</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>117</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>118</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>119</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>120</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>121</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>122</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>123</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>124</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>125</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>126</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>127</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>128</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>129</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>130</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>131</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>132</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>133</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>134</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>135</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>136</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>137</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>138</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>139</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
@@ -2571,7 +2597,7 @@
         <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,7 +2812,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2794,11 +2820,56 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PWCSLMS-23 post processing option
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="Wizard" sheetId="8" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="167">
   <si>
     <t>t</t>
   </si>
@@ -521,37 +521,10 @@
     <t>s</t>
   </si>
   <si>
-    <t>Batch Command</t>
-  </si>
-  <si>
     <t>Gen1P{max,min}</t>
   </si>
   <si>
-    <t>Asim  Copyright (C) 2012, 2013  Power Water Corporation.</t>
-  </si>
-  <si>
-    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
-  </si>
-  <si>
-    <t>This is free software, and you are welcome to redistribute it</t>
-  </si>
-  <si>
-    <t>under certain conditions; see the file COPYING for details.</t>
-  </si>
-  <si>
-    <t>version 2013/06/07-18880</t>
-  </si>
-  <si>
-    <t>Init...</t>
-  </si>
-  <si>
-    <t>Percent Complete</t>
-  </si>
-  <si>
-    <t>Run started on 11/06/2013 4:04:31 PM</t>
-  </si>
-  <si>
-    <t>inner loop took 1.290129s</t>
+    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -822,11 +795,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165102336"/>
-        <c:axId val="165103872"/>
+        <c:axId val="71881856"/>
+        <c:axId val="71883776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165102336"/>
+        <c:axId val="71881856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -838,12 +811,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165103872"/>
+        <c:crossAx val="71883776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165103872"/>
+        <c:axId val="71883776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165102336"/>
+        <c:crossAx val="71881856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -885,6 +858,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -900,9 +877,6 @@
               <c:f>SimResults!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Percent Complete</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -913,9 +887,6 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -930,11 +901,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="35513088"/>
-        <c:axId val="35514624"/>
+        <c:axId val="83956480"/>
+        <c:axId val="83958784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="35513088"/>
+        <c:axId val="83956480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +914,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35514624"/>
+        <c:crossAx val="83958784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -951,7 +922,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35514624"/>
+        <c:axId val="83958784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -964,7 +935,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35513088"/>
+        <c:crossAx val="83956480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,6 +1160,7 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="config"/>
+      <sheetName val="Asim Addin"/>
     </sheetNames>
     <definedNames>
       <definedName name="RunApplication.RunApplication"/>
@@ -1196,6 +1168,7 @@
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1503,9 +1476,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1709,9 +1680,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1807,7 +1776,7 @@
         <v>86400</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1819,6 +1788,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>166</v>
+      </c>
       <c r="B11" s="7" t="s">
         <v>143</v>
       </c>
@@ -1827,9 +1799,6 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>165</v>
-      </c>
       <c r="B12" s="7"/>
     </row>
   </sheetData>
@@ -2812,7 +2781,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2823,53 +2792,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>172</v>
-      </c>
-    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>175</v>
-      </c>
+      <c r="B10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed macros to remove specific reference to users/iain.buchanan
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -795,11 +795,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71881856"/>
-        <c:axId val="71883776"/>
+        <c:axId val="61366656"/>
+        <c:axId val="61368576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71881856"/>
+        <c:axId val="61366656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -811,12 +811,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71883776"/>
+        <c:crossAx val="61368576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71883776"/>
+        <c:axId val="61368576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71881856"/>
+        <c:crossAx val="61366656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -859,7 +859,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -901,11 +900,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="83956480"/>
-        <c:axId val="83958784"/>
+        <c:axId val="86674432"/>
+        <c:axId val="88355200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83956480"/>
+        <c:axId val="86674432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,7 +913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83958784"/>
+        <c:crossAx val="88355200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -922,7 +921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83958784"/>
+        <c:axId val="88355200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -935,7 +934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83956480"/>
+        <c:crossAx val="86674432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1160,7 +1159,6 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="config"/>
-      <sheetName val="Asim Addin"/>
     </sheetNames>
     <definedNames>
       <definedName name="RunApplication.RunApplication"/>
@@ -1168,7 +1166,6 @@
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>

<commit_message>
PWCSLMS-44 changed sheddable load fixed values to parameters
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iain.buchanan\workProjects\pwc.asim.git\PWC.Asim\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725"/>
   </bookViews>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="169">
   <si>
     <t>t</t>
   </si>
@@ -525,6 +530,12 @@
   </si>
   <si>
     <t>Template</t>
+  </si>
+  <si>
+    <t>ShedOffPct</t>
+  </si>
+  <si>
+    <t>ShedOnPct</t>
   </si>
 </sst>
 </file>
@@ -680,6 +691,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -687,7 +701,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -718,6 +732,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -795,11 +810,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61366656"/>
-        <c:axId val="61368576"/>
+        <c:axId val="-851172784"/>
+        <c:axId val="-851172240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61366656"/>
+        <c:axId val="-851172784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -811,12 +826,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61368576"/>
+        <c:crossAx val="-851172240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61368576"/>
+        <c:axId val="-851172240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +842,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61366656"/>
+        <c:crossAx val="-851172784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -847,7 +862,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -900,11 +915,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="86674432"/>
-        <c:axId val="88355200"/>
+        <c:axId val="-851164080"/>
+        <c:axId val="-851171696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86674432"/>
+        <c:axId val="-851164080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +928,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88355200"/>
+        <c:crossAx val="-851171696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -921,7 +936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88355200"/>
+        <c:axId val="-851171696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -934,7 +949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86674432"/>
+        <c:crossAx val="-851164080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,7 +1002,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -995,6 +1010,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
@@ -1012,7 +1033,6 @@
                 </a:rPr>
                 <a:t>Run Wizard</a:t>
               </a:r>
-              <a:endParaRPr lang="en-AU"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -1047,7 +1067,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1055,6 +1075,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
@@ -1072,7 +1098,6 @@
                 </a:rPr>
                 <a:t>Run Asim</a:t>
               </a:r>
-              <a:endParaRPr lang="en-AU"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -1226,7 +1251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1261,7 +1286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2540,19 +2565,19 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2565,8 +2590,14 @@
       <c r="D1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2578,6 +2609,12 @@
       </c>
       <c r="D2">
         <v>1</v>
+      </c>
+      <c r="E2">
+        <v>99</v>
+      </c>
+      <c r="F2">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the buttons from the Wizard. Cleaned up the config page so that it now only has references to files that exist in the install. Added the Run Wizard button to the Addin menu. Made sure that the Addin menu always loads. Added the load.zip which contains the load data.
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iain.buchanan\workProjects\pwc.asim.git\PWC.Asim\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\git.pwc.asim\PWC.Asim\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="166">
   <si>
     <t>t</t>
   </si>
@@ -457,12 +457,6 @@
     <t>load.csv</t>
   </si>
   <si>
-    <t>renewables.csv</t>
-  </si>
-  <si>
-    <t>NPV Analyser.xls</t>
-  </si>
-  <si>
     <t>GenAvailSet</t>
   </si>
   <si>
@@ -478,12 +472,6 @@
     <t>Simulator</t>
   </si>
   <si>
-    <t>bin\Asim.exe</t>
-  </si>
-  <si>
-    <t>bin\AsimExcelTools.exe</t>
-  </si>
-  <si>
     <t>Hysteresis</t>
   </si>
   <si>
@@ -529,13 +517,16 @@
     <t>Gen1P{max,min}</t>
   </si>
   <si>
-    <t>Template</t>
-  </si>
-  <si>
     <t>ShedOffPct</t>
   </si>
   <si>
     <t>ShedOnPct</t>
+  </si>
+  <si>
+    <t>..\bin\AsimExcelTools.exe</t>
+  </si>
+  <si>
+    <t>..\bin\Asim.exe</t>
   </si>
 </sst>
 </file>
@@ -545,7 +536,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,12 +565,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -651,7 +636,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
@@ -660,6 +645,18 @@
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -671,18 +668,6 @@
         <color theme="1" tint="0.499984740745262"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
       </font>
     </dxf>
   </dxfs>
@@ -732,7 +717,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -810,11 +794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-851172784"/>
-        <c:axId val="-851172240"/>
+        <c:axId val="-1549063152"/>
+        <c:axId val="-1549054992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-851172784"/>
+        <c:axId val="-1549063152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -826,12 +810,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-851172240"/>
+        <c:crossAx val="-1549054992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-851172240"/>
+        <c:axId val="-1549054992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-851172784"/>
+        <c:crossAx val="-1549063152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -915,11 +899,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-851164080"/>
-        <c:axId val="-851171696"/>
+        <c:axId val="-1549059344"/>
+        <c:axId val="-1549054448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-851164080"/>
+        <c:axId val="-1549059344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,7 +912,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-851171696"/>
+        <c:crossAx val="-1549054448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -936,7 +920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-851171696"/>
+        <c:axId val="-1549054448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -949,7 +933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-851164080"/>
+        <c:crossAx val="-1549059344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -966,150 +950,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3073" name="RunWizard" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s3073"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Calibri"/>
-                </a:rPr>
-                <a:t>Run Wizard</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>552450</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3075" name="RunAsim" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s3075"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Calibri"/>
-                </a:rPr>
-                <a:t>Run Asim</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1144,7 +985,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1184,6 +1025,7 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="config"/>
+      <sheetName val="Asim Addin"/>
     </sheetNames>
     <definedNames>
       <definedName name="RunApplication.RunApplication"/>
@@ -1191,6 +1033,7 @@
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1199,7 +1042,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:D11" totalsRowShown="0" headerRowCellStyle="60% - Accent1">
   <tableColumns count="4">
-    <tableColumn id="1" name="Parameter" dataDxfId="0"/>
+    <tableColumn id="1" name="Parameter" dataDxfId="2"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Value"/>
     <tableColumn id="4" name="Units"/>
@@ -1494,11 +1337,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1509,7 +1354,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1517,16 +1362,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1534,13 +1379,13 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C5">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,13 +1393,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C6">
         <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,13 +1407,13 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C7">
         <v>3600</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,13 +1421,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C8">
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,13 +1435,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,13 +1449,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,81 +1463,29 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C11">
         <v>400</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",F1)))</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
       <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="3073" r:id="rId4" name="RunWizard">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!StartupWizard.RunWizard">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
-                    <xdr:row>13</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="3075" r:id="rId5" name="RunAsim">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!RunApplication.RunApplication">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>552450</xdr:colOff>
-                    <xdr:row>13</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1700,9 +1493,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1725,19 +1520,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1747,7 +1542,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>140</v>
@@ -1781,57 +1576,38 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>142</v>
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>86400</v>
+      </c>
+      <c r="D8" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9">
-        <v>86400</v>
-      </c>
-      <c r="D9" t="s">
-        <v>165</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
+      <c r="B10" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A5">
       <formula1>",,,,,,,,input,output,Start Time,Community Name"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B9">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A4">
@@ -1840,16 +1616,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2">
       <formula1>",,,,,Community Name,,,input,output,,FlattenApplication"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A8">
       <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter,output"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
-      <formula1>",,,,,Community Name,,Log File,input,output,,Watch,Parameter,Template"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A10">
       <formula1>",,,,,Community Name,Template,Log File,input,output,,Watch,Parameter,Batch Command"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1905,7 +1678,7 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>15</v>
@@ -2588,13 +2361,13 @@
         <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Saved the Example.xls so that it is now the same as the xlsx file.
</commit_message>
<xml_diff>
--- a/PWC.Asim/Data/Example.xlsx
+++ b/PWC.Asim/Data/Example.xlsx
@@ -21,9 +21,6 @@
     <sheet name="Solar" sheetId="5" r:id="rId7"/>
     <sheet name="SimResults" sheetId="6" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -647,18 +644,6 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -668,6 +653,18 @@
         <color theme="1" tint="0.499984740745262"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
       </font>
     </dxf>
   </dxfs>
@@ -794,11 +791,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1549063152"/>
-        <c:axId val="-1549054992"/>
+        <c:axId val="-1035416560"/>
+        <c:axId val="-1035413840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1549063152"/>
+        <c:axId val="-1035416560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -810,12 +807,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1549054992"/>
+        <c:crossAx val="-1035413840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1549054992"/>
+        <c:axId val="-1035413840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1549063152"/>
+        <c:crossAx val="-1035416560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -899,11 +896,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1549059344"/>
-        <c:axId val="-1549054448"/>
+        <c:axId val="-1035412752"/>
+        <c:axId val="-1035418736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1549059344"/>
+        <c:axId val="-1035412752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,7 +909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1549054448"/>
+        <c:crossAx val="-1035418736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -920,7 +917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1549054448"/>
+        <c:axId val="-1035418736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -933,7 +930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1549059344"/>
+        <c:crossAx val="-1035412752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1020,29 +1017,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="config"/>
-      <sheetName val="Asim Addin"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="RunApplication.RunApplication"/>
-      <definedName name="StartupWizard.RunWizard"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:D11" totalsRowShown="0" headerRowCellStyle="60% - Accent1">
   <tableColumns count="4">
-    <tableColumn id="1" name="Parameter" dataDxfId="2"/>
+    <tableColumn id="1" name="Parameter" dataDxfId="0"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Value"/>
     <tableColumn id="4" name="Units"/>
@@ -1341,9 +1319,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1475,10 +1451,10 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>